<commit_message>
Initial commit - safe version without credentials
</commit_message>
<xml_diff>
--- a/output/health_table.xlsx
+++ b/output/health_table.xlsx
@@ -526,27 +526,27 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>202 / 4,901</t>
+          <t>203 / 4,901</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>6,497,422</t>
+          <t>6,503,000</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>8,627,290</t>
+          <t>8,670,609</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>43,202</t>
+          <t>30,540</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -556,12 +556,12 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>263,368</t>
+          <t>265,592</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>07-24 14:45</t>
+          <t>07-24 15:27</t>
         </is>
       </c>
       <c r="M3" t="inlineStr"/>
@@ -594,37 +594,37 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>61 / 5,094</t>
+          <t>63 / 5,093</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>1,809,884</t>
+          <t>1,907,128</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>113,669</t>
+          <t>129,884</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2,853</t>
+          <t>2,923</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2,130</t>
+          <t>2,139</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>174,435</t>
+          <t>174,417</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>07-24 14:45</t>
+          <t>07-24 15:27</t>
         </is>
       </c>
       <c r="M4" t="inlineStr"/>
@@ -652,27 +652,27 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>192 / 6,788</t>
+          <t>195 / 6,788</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>965,764</t>
+          <t>1,000,898</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>1,368,550</t>
+          <t>1,443,566</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>1,676</t>
+          <t>8,032</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -682,12 +682,12 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>334,007</t>
+          <t>333,297</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>07-24 14:45</t>
+          <t>07-24 15:28</t>
         </is>
       </c>
       <c r="M5" t="inlineStr"/>
@@ -715,7 +715,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>874</t>
+          <t>1,314</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -725,32 +725,32 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>5,764,971</t>
+          <t>5,788,217</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>1,136,710</t>
+          <t>1,173,326</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>872</t>
+          <t>1,442</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>4,006</t>
+          <t>4,016</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>148,766</t>
+          <t>148,689</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>07-24 14:31</t>
+          <t>07-24 15:18</t>
         </is>
       </c>
       <c r="M6" t="inlineStr"/>
@@ -788,32 +788,32 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>132,711</t>
+          <t>175,229</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>49,643</t>
+          <t>57,499</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>505</t>
+          <t>1,025</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>15,203</t>
+          <t>15,208</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>179,226</t>
+          <t>179,215</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>07-24 14:39</t>
+          <t>07-24 15:21</t>
         </is>
       </c>
       <c r="M7" t="inlineStr"/>
@@ -841,42 +841,42 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>618</t>
+          <t>593</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>75 / 5,188</t>
+          <t>77 / 5,188</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>906,690</t>
+          <t>921,233</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>1,807,794</t>
+          <t>1,836,341</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>1,028</t>
+          <t>1,435</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>119</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>25,541</t>
+          <t>25,476</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>07-24 14:39</t>
+          <t>07-24 15:22</t>
         </is>
       </c>
       <c r="M8" t="inlineStr"/>
@@ -904,7 +904,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>181</t>
+          <t>96</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -914,17 +914,17 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>315,712</t>
+          <t>336,331</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>232,895</t>
+          <t>245,940</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>5,768</t>
+          <t>427</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -934,12 +934,12 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>21,304</t>
+          <t>21,457</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>07-24 14:44</t>
+          <t>07-24 15:28</t>
         </is>
       </c>
       <c r="M9" t="inlineStr"/>
@@ -967,42 +967,42 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>25 / 2,500</t>
+          <t>24 / 2,500</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>7,760,983</t>
+          <t>7,820,442</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>7,030,915</t>
+          <t>7,066,519</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1,157,082</t>
+          <t>333,258</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>293</t>
+          <t>299</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>187,126</t>
+          <t>204,255</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>07-24 14:45</t>
+          <t>07-24 15:27</t>
         </is>
       </c>
       <c r="M10" t="inlineStr"/>
@@ -1035,22 +1035,22 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>12 / 1,621</t>
+          <t>3 / 1,621</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>9,237,897</t>
+          <t>9,280,123</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>1,491,728</t>
+          <t>1,511,124</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>9,069</t>
+          <t>5,317</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1060,12 +1060,12 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>73,428</t>
+          <t>73,477</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>07-24 14:45</t>
+          <t>07-24 15:27</t>
         </is>
       </c>
       <c r="M11" t="inlineStr"/>
@@ -1098,22 +1098,22 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>5 / 1,383</t>
+          <t>15 / 1,378</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>1,001,930</t>
+          <t>1,004,118</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>536,421</t>
+          <t>540,008</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>3,542</t>
+          <t>591</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1123,12 +1123,12 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>13,787</t>
+          <t>13,743</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>07-24 14:45</t>
+          <t>07-24 15:27</t>
         </is>
       </c>
       <c r="M12" t="inlineStr"/>
@@ -1171,12 +1171,12 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>520,958</t>
+          <t>521,343</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>7,953</t>
+          <t>16</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1186,12 +1186,12 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>39,004</t>
+          <t>39,056</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>07-24 14:45</t>
+          <t>07-24 15:27</t>
         </is>
       </c>
       <c r="M13" t="inlineStr"/>
@@ -1229,17 +1229,17 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>179,646</t>
+          <t>179,669</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>35,900</t>
+          <t>36,396</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>30</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1249,12 +1249,12 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>6,506</t>
+          <t>6,498</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>07-24 14:45</t>
+          <t>07-24 15:27</t>
         </is>
       </c>
       <c r="M14" t="inlineStr"/>
@@ -1262,7 +1262,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>rossmann-pl</t>
+          <t>rossmann-de</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1287,37 +1287,37 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>6 / 507</t>
+          <t>407</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>58,591</t>
+          <t>72,156</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>19,342</t>
+          <t>441,075</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>174</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>938</t>
+          <t>10,210</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>07-24 14:45</t>
+          <t>07-24 15:27</t>
         </is>
       </c>
       <c r="M15" t="inlineStr"/>
@@ -1325,7 +1325,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>rossmann-de</t>
+          <t>rossmann-pl</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1350,37 +1350,37 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>389</t>
+          <t>6 / 483</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>69,905</t>
+          <t>56,039</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>437,099</t>
+          <t>18,884</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>11</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>24</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>9,796</t>
+          <t>894</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>07-24 14:45</t>
+          <t>07-24 15:27</t>
         </is>
       </c>
       <c r="M16" t="inlineStr"/>
@@ -1408,7 +1408,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>287</t>
+          <t>267</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1418,17 +1418,17 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>76,916</t>
+          <t>77,168</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>41,360</t>
+          <t>41,444</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1443,7 +1443,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>07-24 14:45</t>
+          <t>07-24 15:27</t>
         </is>
       </c>
       <c r="M17" t="inlineStr"/>
@@ -1471,7 +1471,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>35</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1481,17 +1481,17 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2,044,612</t>
+          <t>2,439,136</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>480,775</t>
+          <t>518,300</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>2,314</t>
+          <t>1,640</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1501,12 +1501,12 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>6,892</t>
+          <t>6,856</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>07-24 14:45</t>
+          <t>07-24 15:27</t>
         </is>
       </c>
       <c r="M18" t="inlineStr"/>
@@ -1544,17 +1544,17 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>136,751</t>
+          <t>137,454</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>63,157</t>
+          <t>63,637</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -1569,7 +1569,7 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>07-24 14:44</t>
+          <t>07-24 15:26</t>
         </is>
       </c>
       <c r="M19" t="inlineStr"/>
@@ -1597,29 +1597,29 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>18 / 219</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>429,937</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>135,321</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
           <t>31</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>22 / 219</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>413,089</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>121,094</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
       <c r="J20" t="inlineStr">
         <is>
           <t>537</t>
@@ -1627,12 +1627,12 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>6,493</t>
+          <t>6,489</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>07-24 14:45</t>
+          <t>07-24 15:27</t>
         </is>
       </c>
       <c r="M20" t="inlineStr"/>
@@ -1665,37 +1665,37 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>1 / 490</t>
+          <t>2 / 490</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>207,899</t>
+          <t>208,169</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>10,719</t>
+          <t>11,599</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>614</t>
+          <t>563</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>63</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>22,587</t>
+          <t>22,579</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>07-24 14:45</t>
+          <t>07-24 15:27</t>
         </is>
       </c>
       <c r="M21" t="inlineStr"/>
@@ -1733,17 +1733,17 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>289,697</t>
+          <t>324,985</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>153,698</t>
+          <t>163,932</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>111</t>
+          <t>142</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -1753,12 +1753,12 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>1,444</t>
+          <t>1,385</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>07-24 14:45</t>
+          <t>07-24 15:27</t>
         </is>
       </c>
       <c r="M22" t="inlineStr"/>
@@ -1801,12 +1801,12 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>37,499</t>
+          <t>37,702</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>117</t>
+          <t>56</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -1816,12 +1816,12 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2,907</t>
+          <t>2,959</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>07-24 14:44</t>
+          <t>07-24 15:26</t>
         </is>
       </c>
       <c r="M23" t="inlineStr"/>
@@ -1854,7 +1854,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>8 / 324</t>
+          <t>9 / 324</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1864,12 +1864,12 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>54,498</t>
+          <t>54,612</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>239</t>
+          <t>220</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -1879,12 +1879,12 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>17,436</t>
+          <t>17,454</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>07-24 14:45</t>
+          <t>07-24 15:27</t>
         </is>
       </c>
       <c r="M24" t="inlineStr"/>
@@ -1922,17 +1922,17 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>1,774,447</t>
+          <t>1,774,562</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>1,077</t>
+          <t>1,292</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>9</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -1947,7 +1947,7 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>07-24 14:44</t>
+          <t>07-24 15:26</t>
         </is>
       </c>
       <c r="M25" t="inlineStr"/>
@@ -1985,17 +1985,17 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>146,621</t>
+          <t>147,548</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>144,078</t>
+          <t>145,012</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>1,006</t>
+          <t>989</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -2005,12 +2005,12 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>5,511</t>
+          <t>5,259</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>07-24 14:44</t>
+          <t>07-24 15:26</t>
         </is>
       </c>
       <c r="M26" t="inlineStr"/>
@@ -2048,17 +2048,17 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>625</t>
+          <t>671</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1,047</t>
+          <t>1,106</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2073,7 +2073,7 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>07-24 14:44</t>
+          <t>07-24 15:26</t>
         </is>
       </c>
       <c r="M27" t="inlineStr"/>
@@ -2111,17 +2111,17 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>5,844</t>
+          <t>5,925</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>4,828</t>
+          <t>4,920</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -2131,12 +2131,12 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>1,182</t>
+          <t>1,181</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>07-24 14:44</t>
+          <t>07-24 15:26</t>
         </is>
       </c>
       <c r="M28" t="inlineStr"/>
@@ -2179,12 +2179,12 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>4,393</t>
+          <t>4,440</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -2194,12 +2194,12 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>764</t>
+          <t>785</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>07-24 14:44</t>
+          <t>07-24 15:26</t>
         </is>
       </c>
       <c r="M29" t="inlineStr"/>
@@ -2237,12 +2237,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>179,624</t>
+          <t>202,136</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>804</t>
+          <t>900</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2262,7 +2262,7 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>07-24 14:44</t>
+          <t>07-24 15:26</t>
         </is>
       </c>
       <c r="M30" t="inlineStr"/>
@@ -2290,7 +2290,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2300,17 +2300,17 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>2,498</t>
+          <t>2,764</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>80,159</t>
+          <t>80,329</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -2320,12 +2320,12 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>203</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>07-24 14:44</t>
+          <t>07-24 15:26</t>
         </is>
       </c>
       <c r="M31" t="inlineStr"/>
@@ -2368,7 +2368,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>12,636</t>
+          <t>12,637</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2383,12 +2383,12 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>136</t>
+          <t>135</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>07-24 14:44</t>
+          <t>07-24 15:26</t>
         </is>
       </c>
       <c r="M32" t="inlineStr"/>
@@ -2431,12 +2431,12 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>3,257</t>
+          <t>3,717</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -2451,7 +2451,7 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>07-24 14:44</t>
+          <t>07-24 15:26</t>
         </is>
       </c>
       <c r="M33" t="inlineStr"/>
@@ -2494,7 +2494,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>705</t>
+          <t>706</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2514,7 +2514,7 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>07-24 14:44</t>
+          <t>07-24 15:26</t>
         </is>
       </c>
       <c r="M34" t="inlineStr"/>
@@ -2552,12 +2552,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>5,544</t>
+          <t>5,776</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>3,586</t>
+          <t>3,650</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2577,7 +2577,7 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>07-24 14:44</t>
+          <t>07-24 15:26</t>
         </is>
       </c>
       <c r="M35" t="inlineStr"/>
@@ -2640,7 +2640,7 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>07-24 14:44</t>
+          <t>07-24 15:26</t>
         </is>
       </c>
       <c r="M36" t="inlineStr"/>
@@ -2766,7 +2766,7 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>07-24 14:39</t>
+          <t>07-24 15:21</t>
         </is>
       </c>
       <c r="M38" t="inlineStr"/>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>07-24 14:44</t>
+          <t>07-24 15:26</t>
         </is>
       </c>
       <c r="M39" t="inlineStr"/>

</xml_diff>